<commit_message>
Updated with new container types
Added binder and sheet to valid container types.
</commit_message>
<xml_diff>
--- a/aspace_import_excel_template (Smith version).xlsx
+++ b/aspace_import_excel_template (Smith version).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17610" windowHeight="8955"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9630"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -1571,9 +1571,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AOA6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2629,7 +2629,7 @@
       <formula1>"accession,audio,books,computer_disks,digital_object,graphic_materials,microform,mixed_materials,moving_images"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE6:AE1048576 AC6:AC1048576 Z6:Z1048576">
-      <formula1>"box,folder,drawer,item,mapcase,microdex,Portfolio,reel,roll,tube"</formula1>
+      <formula1>"box,folder,binder,drawer,item,mapcase,microdex,Portfolio,reel,roll,sheet,tube"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Added volume as container type
</commit_message>
<xml_diff>
--- a/aspace_import_excel_template (Smith version).xlsx
+++ b/aspace_import_excel_template (Smith version).xlsx
@@ -1573,7 +1573,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z7" sqref="Z7"/>
+      <selection pane="bottomLeft" activeCell="Z6" sqref="Z6:Z1048576 AC6:AC1048576 AE6:AE1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2629,7 +2629,7 @@
       <formula1>"accession,audio,books,computer_disks,digital_object,graphic_materials,microform,mixed_materials,moving_images"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z6:Z1048576 AC6:AC1048576 AE6:AE1048576">
-      <formula1>"box,folder,binder,drawer,envelope,flat file folder,item,mapcase,microdex,Portfolio,reel,roll,sheet,tube"</formula1>
+      <formula1>"box,folder,binder,drawer,envelope,flat file folder,item,mapcase,microdex,Portfolio,reel,roll,sheet,tube,volume"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>